<commit_message>
started defining more framework feature stuff, displaying framework features in ui
</commit_message>
<xml_diff>
--- a/docs/features/framework-features.xlsx
+++ b/docs/features/framework-features.xlsx
@@ -178,9 +178,6 @@
     <t>DRGN_TAIL_LASH</t>
   </si>
   <si>
-    <t>The dragon can sweep all opponents in his rear facing in a 2" long by 4" wide rectangle. This is a Fighting attack which ignores size penalties, doing Str+d8 (Mega Damage). DRAGON HATCHLING COMPLICATIONS For all their power, Dragon Hatchlings begin life with a number of limitations and difficulties.</t>
-  </si>
-  <si>
     <t>GB_ENEMIES</t>
   </si>
   <si>
@@ -421,9 +418,6 @@
     <t>DRGN_FORM_LIMITS</t>
   </si>
   <si>
-    <t>If a dragon transforms into a humanoid race with a restriction based on its body type (such as Non- Standard Physiology, see page 51), it suffers the same penalties as that race. The GM m akes t he fi nal c all o n what 47 counts as a body type restriction. In their natural form, dragons cannot wear any armor and can only use vehicular weapons specially adapted for their use at four times the normal cost. Most other gear can only be used in humanoid form (again, GM’s call).</t>
-  </si>
-  <si>
     <t>DRGN_INHERENTLY_MAGICAL</t>
   </si>
   <si>
@@ -866,6 +860,12 @@
   </si>
   <si>
     <t>GADGETEER</t>
+  </si>
+  <si>
+    <t>The dragon can sweep all opponents in his rear facing in a 2" long by 4" wide rectangle. This is a Fighting attack which ignores size penalties, doing Str+d8 (Mega Damage).</t>
+  </si>
+  <si>
+    <t>If a dragon transforms into a humanoid race with a restriction based on its body type (such as Non- Standard Physiology, see page 51), it suffers the same penalties as that race. The GM makes the final c all on what counts as a body type restriction. In their natural form, dragons cannot wear any armor and can only use vehicular weapons specially adapted for their use at four times the normal cost. Most other gear can only be used in humanoid form (again, GM’s call).</t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1210,7 @@
   <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1237,13 +1237,13 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E2" t="str">
         <f>"INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = '"&amp;A2&amp;"'), (SELECT id FROM edge WHERE edge_type = '"&amp;C2&amp;"')); "</f>
@@ -1284,7 +1284,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
@@ -1335,13 +1335,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -1376,13 +1376,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -1414,13 +1414,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -1433,13 +1433,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -1471,13 +1471,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -1490,13 +1490,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -1528,13 +1528,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B17" t="s">
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -1547,13 +1547,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -1566,13 +1566,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -1585,13 +1585,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B20" t="s">
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -1604,13 +1604,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
@@ -1623,13 +1623,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
@@ -1673,7 +1673,7 @@
         <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
@@ -1686,13 +1686,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B25" t="s">
         <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
@@ -1705,13 +1705,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B26" t="s">
         <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
@@ -1724,13 +1724,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
         <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
@@ -1762,13 +1762,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
         <v>106</v>
-      </c>
-      <c r="B29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="s">
-        <v>107</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
@@ -1781,13 +1781,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
       </c>
       <c r="D30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
@@ -1800,13 +1800,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B31" t="s">
         <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
@@ -1819,13 +1819,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
@@ -1838,13 +1838,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B33" t="s">
         <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
@@ -1857,13 +1857,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="D34" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
@@ -1876,16 +1876,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B35" t="s">
         <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
@@ -1898,13 +1898,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
       <c r="D36" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="0"/>
@@ -1917,7 +1917,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B37" t="s">
         <v>11</v>
@@ -1926,7 +1926,7 @@
         <v>6</v>
       </c>
       <c r="D37" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
@@ -1939,13 +1939,13 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B38" t="s">
         <v>11</v>
       </c>
       <c r="D38" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="0"/>
@@ -1958,13 +1958,13 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B39" t="s">
         <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
@@ -1977,13 +1977,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B40" t="s">
         <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
@@ -1996,13 +1996,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B41" t="s">
         <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
@@ -2015,16 +2015,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
@@ -2037,13 +2037,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" t="s">
         <v>78</v>
-      </c>
-      <c r="B43" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" t="s">
-        <v>79</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
@@ -2056,13 +2056,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="D44" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
@@ -2075,13 +2075,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" t="s">
         <v>82</v>
-      </c>
-      <c r="B45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" t="s">
-        <v>83</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
@@ -2094,13 +2094,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B46" t="s">
         <v>14</v>
       </c>
       <c r="D46" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
@@ -2113,13 +2113,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" t="s">
         <v>76</v>
-      </c>
-      <c r="B47" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" t="s">
-        <v>77</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
@@ -2132,13 +2132,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B48" t="s">
         <v>14</v>
       </c>
       <c r="D48" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
@@ -2151,13 +2151,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" t="s">
         <v>55</v>
-      </c>
-      <c r="B49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D49" t="s">
-        <v>56</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
@@ -2170,13 +2170,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" t="s">
         <v>110</v>
-      </c>
-      <c r="B50" t="s">
-        <v>14</v>
-      </c>
-      <c r="D50" t="s">
-        <v>111</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
@@ -2189,13 +2189,13 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
         <v>14</v>
       </c>
       <c r="D51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
@@ -2208,13 +2208,13 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B52" t="s">
         <v>14</v>
       </c>
       <c r="D52" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
@@ -2227,13 +2227,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
         <v>65</v>
-      </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" t="s">
-        <v>66</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
@@ -2246,13 +2246,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B54" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" t="s">
         <v>122</v>
-      </c>
-      <c r="B54" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" t="s">
-        <v>123</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
@@ -2265,7 +2265,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B55" t="s">
         <v>11</v>
@@ -2274,7 +2274,7 @@
         <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
@@ -2287,7 +2287,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B56" t="s">
         <v>11</v>
@@ -2296,7 +2296,7 @@
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
@@ -2309,16 +2309,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" t="s">
+        <v>272</v>
+      </c>
+      <c r="D57" t="s">
         <v>124</v>
-      </c>
-      <c r="B57" t="s">
-        <v>11</v>
-      </c>
-      <c r="C57" t="s">
-        <v>274</v>
-      </c>
-      <c r="D57" t="s">
-        <v>125</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
@@ -2331,13 +2331,13 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B58" t="s">
         <v>14</v>
       </c>
       <c r="D58" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
@@ -2369,13 +2369,13 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>129</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" t="s">
         <v>130</v>
-      </c>
-      <c r="B60" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" t="s">
-        <v>131</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
@@ -2388,13 +2388,13 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" t="s">
         <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>14</v>
-      </c>
-      <c r="D61" t="s">
-        <v>60</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
@@ -2407,13 +2407,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
@@ -2445,13 +2445,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
       </c>
       <c r="D64" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="0"/>
@@ -2464,13 +2464,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" t="s">
         <v>80</v>
-      </c>
-      <c r="B65" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" t="s">
-        <v>81</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="0"/>
@@ -2483,13 +2483,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>60</v>
+      </c>
+      <c r="B66" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
         <v>61</v>
-      </c>
-      <c r="B66" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" t="s">
-        <v>62</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="0"/>
@@ -2502,13 +2502,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
         <v>63</v>
-      </c>
-      <c r="B67" t="s">
-        <v>11</v>
-      </c>
-      <c r="D67" t="s">
-        <v>64</v>
       </c>
       <c r="E67" t="str">
         <f t="shared" ref="E67:E130" si="2">"INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = '"&amp;A67&amp;"'), (SELECT id FROM edge WHERE edge_type = '"&amp;C67&amp;"')); "</f>
@@ -2521,16 +2521,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B68" t="s">
         <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D68" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="2"/>
@@ -2543,13 +2543,13 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>71</v>
+      </c>
+      <c r="B69" t="s">
+        <v>14</v>
+      </c>
+      <c r="D69" t="s">
         <v>72</v>
-      </c>
-      <c r="B69" t="s">
-        <v>14</v>
-      </c>
-      <c r="D69" t="s">
-        <v>73</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="2"/>
@@ -2562,13 +2562,13 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>56</v>
+      </c>
+      <c r="B70" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" t="s">
         <v>57</v>
-      </c>
-      <c r="B70" t="s">
-        <v>14</v>
-      </c>
-      <c r="D70" t="s">
-        <v>58</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="2"/>
@@ -2600,13 +2600,13 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B72" t="s">
         <v>11</v>
       </c>
       <c r="D72" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="2"/>
@@ -2619,13 +2619,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" t="s">
         <v>102</v>
-      </c>
-      <c r="B73" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" t="s">
-        <v>103</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="2"/>
@@ -2638,16 +2638,16 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" t="s">
+        <v>273</v>
+      </c>
+      <c r="D74" t="s">
         <v>100</v>
-      </c>
-      <c r="B74" t="s">
-        <v>11</v>
-      </c>
-      <c r="C74" t="s">
-        <v>275</v>
-      </c>
-      <c r="D74" t="s">
-        <v>101</v>
       </c>
       <c r="E74" t="str">
         <f t="shared" si="2"/>
@@ -2660,16 +2660,16 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
       </c>
       <c r="C75" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D75" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E75" t="str">
         <f t="shared" si="2"/>
@@ -2682,13 +2682,13 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B76" t="s">
         <v>11</v>
       </c>
       <c r="D76" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E76" t="str">
         <f t="shared" si="2"/>
@@ -2720,13 +2720,13 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>85</v>
+      </c>
+      <c r="B78" t="s">
+        <v>14</v>
+      </c>
+      <c r="D78" t="s">
         <v>86</v>
-      </c>
-      <c r="B78" t="s">
-        <v>14</v>
-      </c>
-      <c r="D78" t="s">
-        <v>87</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="2"/>
@@ -2739,13 +2739,13 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>103</v>
+      </c>
+      <c r="B79" t="s">
+        <v>14</v>
+      </c>
+      <c r="D79" t="s">
         <v>104</v>
-      </c>
-      <c r="B79" t="s">
-        <v>14</v>
-      </c>
-      <c r="D79" t="s">
-        <v>105</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="2"/>
@@ -2777,13 +2777,13 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>117</v>
+      </c>
+      <c r="B81" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" t="s">
         <v>118</v>
-      </c>
-      <c r="B81" t="s">
-        <v>11</v>
-      </c>
-      <c r="D81" t="s">
-        <v>119</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="2"/>
@@ -2796,13 +2796,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>115</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" t="s">
         <v>116</v>
-      </c>
-      <c r="B82" t="s">
-        <v>11</v>
-      </c>
-      <c r="D82" t="s">
-        <v>117</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="2"/>
@@ -2815,13 +2815,13 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" t="s">
         <v>112</v>
-      </c>
-      <c r="B83" t="s">
-        <v>11</v>
-      </c>
-      <c r="D83" t="s">
-        <v>113</v>
       </c>
       <c r="E83" t="str">
         <f t="shared" si="2"/>
@@ -2853,13 +2853,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B85" t="s">
         <v>11</v>
       </c>
       <c r="D85" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="2"/>
@@ -2891,13 +2891,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B87" t="s">
         <v>11</v>
       </c>
       <c r="D87" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="2"/>
@@ -2910,16 +2910,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>73</v>
+      </c>
+      <c r="B88" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" t="s">
+        <v>276</v>
+      </c>
+      <c r="D88" t="s">
         <v>74</v>
-      </c>
-      <c r="B88" t="s">
-        <v>11</v>
-      </c>
-      <c r="C88" t="s">
-        <v>278</v>
-      </c>
-      <c r="D88" t="s">
-        <v>75</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="2"/>
@@ -2932,16 +2932,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>73</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" t="s">
+        <v>278</v>
+      </c>
+      <c r="D89" t="s">
         <v>74</v>
-      </c>
-      <c r="B89" t="s">
-        <v>11</v>
-      </c>
-      <c r="C89" t="s">
-        <v>280</v>
-      </c>
-      <c r="D89" t="s">
-        <v>75</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="2"/>
@@ -2954,13 +2954,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>69</v>
+      </c>
+      <c r="B90" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" t="s">
         <v>70</v>
-      </c>
-      <c r="B90" t="s">
-        <v>14</v>
-      </c>
-      <c r="D90" t="s">
-        <v>71</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="2"/>
@@ -2973,13 +2973,13 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>113</v>
+      </c>
+      <c r="B91" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" t="s">
         <v>114</v>
-      </c>
-      <c r="B91" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" t="s">
-        <v>115</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="2"/>
@@ -2992,13 +2992,13 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B92" t="s">
         <v>14</v>
       </c>
       <c r="D92" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="2"/>
@@ -3011,16 +3011,16 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93" t="s">
+        <v>275</v>
+      </c>
+      <c r="D93" t="s">
         <v>96</v>
-      </c>
-      <c r="B93" t="s">
-        <v>11</v>
-      </c>
-      <c r="C93" t="s">
-        <v>277</v>
-      </c>
-      <c r="D93" t="s">
-        <v>97</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="2"/>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B94" t="s">
         <v>11</v>
@@ -3042,7 +3042,7 @@
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="2"/>
@@ -3055,13 +3055,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>83</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" t="s">
         <v>84</v>
-      </c>
-      <c r="B95" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" t="s">
-        <v>85</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="2"/>
@@ -3074,16 +3074,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>89</v>
+      </c>
+      <c r="B96" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96" t="s">
+        <v>276</v>
+      </c>
+      <c r="D96" t="s">
         <v>90</v>
-      </c>
-      <c r="B96" t="s">
-        <v>11</v>
-      </c>
-      <c r="C96" t="s">
-        <v>278</v>
-      </c>
-      <c r="D96" t="s">
-        <v>91</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="2"/>
@@ -3096,16 +3096,16 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>89</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" t="s">
+        <v>278</v>
+      </c>
+      <c r="D97" t="s">
         <v>90</v>
-      </c>
-      <c r="B97" t="s">
-        <v>11</v>
-      </c>
-      <c r="C97" t="s">
-        <v>280</v>
-      </c>
-      <c r="D97" t="s">
-        <v>91</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="2"/>
@@ -3118,16 +3118,16 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>91</v>
+      </c>
+      <c r="B98" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" t="s">
+        <v>279</v>
+      </c>
+      <c r="D98" t="s">
         <v>92</v>
-      </c>
-      <c r="B98" t="s">
-        <v>11</v>
-      </c>
-      <c r="C98" t="s">
-        <v>281</v>
-      </c>
-      <c r="D98" t="s">
-        <v>93</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="2"/>
@@ -3140,16 +3140,16 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>91</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" t="s">
+        <v>280</v>
+      </c>
+      <c r="D99" t="s">
         <v>92</v>
-      </c>
-      <c r="B99" t="s">
-        <v>11</v>
-      </c>
-      <c r="C99" t="s">
-        <v>282</v>
-      </c>
-      <c r="D99" t="s">
-        <v>93</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="2"/>
@@ -3162,13 +3162,13 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B100" t="s">
         <v>11</v>
       </c>
       <c r="D100" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="2"/>
@@ -3181,13 +3181,13 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>93</v>
+      </c>
+      <c r="B101" t="s">
+        <v>14</v>
+      </c>
+      <c r="D101" t="s">
         <v>94</v>
-      </c>
-      <c r="B101" t="s">
-        <v>14</v>
-      </c>
-      <c r="D101" t="s">
-        <v>95</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="2"/>
@@ -3200,13 +3200,13 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>87</v>
+      </c>
+      <c r="B102" t="s">
+        <v>14</v>
+      </c>
+      <c r="D102" t="s">
         <v>88</v>
-      </c>
-      <c r="B102" t="s">
-        <v>14</v>
-      </c>
-      <c r="D102" t="s">
-        <v>89</v>
       </c>
       <c r="E102" t="str">
         <f t="shared" si="2"/>
@@ -3219,13 +3219,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>97</v>
+      </c>
+      <c r="B103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" t="s">
         <v>98</v>
-      </c>
-      <c r="B103" t="s">
-        <v>14</v>
-      </c>
-      <c r="D103" t="s">
-        <v>99</v>
       </c>
       <c r="E103" t="str">
         <f t="shared" si="2"/>
@@ -3238,13 +3238,13 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B104" t="s">
         <v>14</v>
       </c>
       <c r="D104" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" si="2"/>
@@ -3257,16 +3257,16 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>66</v>
+      </c>
+      <c r="B105" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105" t="s">
+        <v>277</v>
+      </c>
+      <c r="D105" t="s">
         <v>67</v>
-      </c>
-      <c r="B105" t="s">
-        <v>11</v>
-      </c>
-      <c r="C105" t="s">
-        <v>279</v>
-      </c>
-      <c r="D105" t="s">
-        <v>68</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="2"/>
@@ -3279,13 +3279,13 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B106" t="s">
         <v>11</v>
       </c>
       <c r="C106" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D106" t="s">
         <v>8</v>
@@ -3301,13 +3301,13 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B107" t="s">
         <v>11</v>
       </c>
       <c r="D107" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="2"/>
@@ -3320,13 +3320,13 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B108" t="s">
         <v>11</v>
       </c>
       <c r="D108" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="2"/>
@@ -3339,13 +3339,13 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B109" t="s">
         <v>14</v>
       </c>
       <c r="D109" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="2"/>
@@ -3358,13 +3358,13 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B110" t="s">
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="2"/>
@@ -3377,13 +3377,13 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>107</v>
+      </c>
+      <c r="B111" t="s">
+        <v>14</v>
+      </c>
+      <c r="D111" t="s">
         <v>108</v>
-      </c>
-      <c r="B111" t="s">
-        <v>14</v>
-      </c>
-      <c r="D111" t="s">
-        <v>109</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="2"/>
@@ -3415,7 +3415,7 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B113" t="s">
         <v>11</v>
@@ -3424,7 +3424,7 @@
         <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="2"/>
@@ -3456,13 +3456,13 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B115" t="s">
         <v>11</v>
       </c>
       <c r="D115" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E115" t="str">
         <f t="shared" si="2"/>
@@ -3475,13 +3475,13 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>131</v>
+      </c>
+      <c r="B116" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" t="s">
         <v>132</v>
-      </c>
-      <c r="B116" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116" t="s">
-        <v>133</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="2"/>
@@ -3494,13 +3494,13 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B117" t="s">
         <v>11</v>
       </c>
       <c r="D117" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="2"/>
@@ -3532,13 +3532,13 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B119" t="s">
         <v>11</v>
       </c>
       <c r="D119" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="2"/>
@@ -3551,13 +3551,13 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B120" t="s">
         <v>11</v>
       </c>
       <c r="D120" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="2"/>
@@ -3570,13 +3570,13 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B121" t="s">
         <v>11</v>
       </c>
       <c r="D121" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="2"/>
@@ -3589,13 +3589,13 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B122" t="s">
         <v>11</v>
       </c>
       <c r="D122" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E122" t="str">
         <f t="shared" si="2"/>
@@ -3608,13 +3608,13 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B123" t="s">
         <v>11</v>
       </c>
       <c r="D123" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E123" t="str">
         <f t="shared" si="2"/>
@@ -3646,13 +3646,13 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>127</v>
+      </c>
+      <c r="B125" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" t="s">
         <v>128</v>
-      </c>
-      <c r="B125" t="s">
-        <v>11</v>
-      </c>
-      <c r="D125" t="s">
-        <v>129</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="2"/>
@@ -3690,90 +3690,82 @@
         <v>11</v>
       </c>
       <c r="D127" t="s">
-        <v>54</v>
+        <v>282</v>
       </c>
       <c r="E127" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_TAIL_LASH'), (SELECT id FROM edge WHERE edge_type = '')); </v>
       </c>
       <c r="F127" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f>"UPDATE `framework_feature` SET description='"&amp;D127&amp;"' WHERE framework_ability_type = '"&amp;A127&amp;"'; "</f>
+        <v xml:space="preserve">UPDATE `framework_feature` SET description='The dragon can sweep all opponents in his rear facing in a 2" long by 4" wide rectangle. This is a Fighting attack which ignores size penalties, doing Str+d8 (Mega Damage).' WHERE framework_ability_type = 'DRGN_TAIL_LASH'; </v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B128" t="s">
         <v>14</v>
       </c>
       <c r="D128" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E128" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_CYBERNETICS'), (SELECT id FROM edge WHERE edge_type = '')); </v>
-      </c>
-      <c r="F128" t="str">
-        <f t="shared" si="3"/>
-        <v/>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B129" t="s">
         <v>14</v>
       </c>
       <c r="D129" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E129" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_ENEMIES'), (SELECT id FROM edge WHERE edge_type = '')); </v>
-      </c>
-      <c r="F129" t="str">
-        <f t="shared" si="3"/>
-        <v/>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B130" t="s">
         <v>14</v>
       </c>
       <c r="D130" t="s">
-        <v>135</v>
+        <v>283</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_FORM_LIMITS'), (SELECT id FROM edge WHERE edge_type = '')); </v>
       </c>
       <c r="F130" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+        <f t="shared" ref="F128:F130" si="4">"UPDATE `framework_feature` SET description='"&amp;D130&amp;"' WHERE framework_ability_type = '"&amp;A130&amp;"'; "</f>
+        <v xml:space="preserve">UPDATE `framework_feature` SET description='If a dragon transforms into a humanoid race with a restriction based on its body type (such as Non- Standard Physiology, see page 51), it suffers the same penalties as that race. The GM makes the final c all on what counts as a body type restriction. In their natural form, dragons cannot wear any armor and can only use vehicular weapons specially adapted for their use at four times the normal cost. Most other gear can only be used in humanoid form (again, GM’s call).' WHERE framework_ability_type = 'DRGN_FORM_LIMITS'; </v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B131" t="s">
         <v>14</v>
       </c>
       <c r="D131" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" ref="E131:E137" si="4">"INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = '"&amp;A131&amp;"'), (SELECT id FROM edge WHERE edge_type = '"&amp;C131&amp;"')); "</f>
+        <f t="shared" ref="E131:E136" si="5">"INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = '"&amp;A131&amp;"'), (SELECT id FROM edge WHERE edge_type = '"&amp;C131&amp;"')); "</f>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_HATCHED'), (SELECT id FROM edge WHERE edge_type = '')); </v>
       </c>
       <c r="F131" t="str">
-        <f t="shared" ref="F131:F136" si="5">IF(ISBLANK(C131), "", E131)</f>
+        <f t="shared" ref="F131:F136" si="6">IF(ISBLANK(C131), "", E131)</f>
         <v/>
       </c>
     </row>
@@ -3788,91 +3780,92 @@
         <v>27</v>
       </c>
       <c r="E132" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_LARGE'), (SELECT id FROM edge WHERE edge_type = '')); </v>
       </c>
       <c r="F132" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B133" t="s">
         <v>14</v>
       </c>
       <c r="D133" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E133" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_OUTSIDER'), (SELECT id FROM edge WHERE edge_type = '')); </v>
       </c>
       <c r="F133" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B134" t="s">
         <v>14</v>
       </c>
       <c r="D134" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E134" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_TERRITORIAL'), (SELECT id FROM edge WHERE edge_type = '')); </v>
       </c>
       <c r="F134" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B135" t="s">
         <v>14</v>
       </c>
       <c r="D135" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E135" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_UNTESTED'), (SELECT id FROM edge WHERE edge_type = '')); </v>
       </c>
       <c r="F135" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B136" t="s">
         <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E136" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">INSERT INTO `framework_edge` (framework_feature, edge) VALUES ((SELECT id FROM framework_feature WHERE framework_feature_type = 'DRGN_VERY_YOUNG'), (SELECT id FROM edge WHERE edge_type = '')); </v>
       </c>
       <c r="F136" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>